<commit_message>
Separated data into CSVs for visualisation
</commit_message>
<xml_diff>
--- a/Analysis/decision_analysis.xlsx
+++ b/Analysis/decision_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yakir/Documents/Monash University/2023 S1/FIT3164 Data science project 2/fit3164-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yakir/Documents/Monash University/2023 S1/FIT3164 Data science project 2/fit3164-project/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EED5520-5BC4-7E4B-A7A0-13C3AD38519A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CF5287-3AF1-B149-A4C1-A32B5AEB458B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{C9331C5C-3E1B-1149-BFFD-5499CEEBA534}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{C9331C5C-3E1B-1149-BFFD-5499CEEBA534}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,27 +18,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$93</definedName>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$E$55:$E$59</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$F$54</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet2!$G$3:$G$6</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet2!$E$55:$E$59</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet2!$F$54</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet2!$F$55:$F$59</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet2!$E$37:$E$41</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet2!$F$36</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet2!$F$37:$F$41</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$F$55:$F$59</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$F$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$F$3:$F$6</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet2!$G$2</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet2!$G$3:$G$6</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet2!$F$2</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet2!$F$3:$F$6</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet2!$G$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6197,177 +6180,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{478BA645-ED55-2142-8FD5-ECA1AB24B187}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Quarter">
-  <location ref="A1:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" showAll="0" sortType="descending">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Classification" fld="15" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{982984A0-7D40-CC4A-94E5-14BF1B036463}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Average_Pressure">
-  <location ref="A53:C59" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="2" showAll="0"/>
-    <pivotField numFmtId="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" showAll="0" sortType="descending">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="15"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Classification" fld="15" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6994B56D-9B22-7947-8941-05595B5C1D53}" name="PivotTable8" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Effectiveness">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6994B56D-9B22-7947-8941-05595B5C1D53}" name="PivotTable8" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Effectiveness">
   <location ref="A35:C41" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -6458,8 +6271,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CAA60AE6-0C3E-8448-9887-83353A6E0B0F}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Round">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CAA60AE6-0C3E-8448-9887-83353A6E0B0F}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Round">
   <location ref="A17:C24" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0"/>
@@ -6516,6 +6329,176 @@
     </i>
     <i>
       <x v="5"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Classification" fld="15" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{478BA645-ED55-2142-8FD5-ECA1AB24B187}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Quarter">
+  <location ref="A1:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" showAll="0" sortType="descending">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="15"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Classification" fld="15" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{982984A0-7D40-CC4A-94E5-14BF1B036463}" name="PivotTable9" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Average_Pressure">
+  <location ref="A53:C59" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" showAll="0" sortType="descending">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
   </rowItems>
   <colFields count="1">
@@ -6843,9 +6826,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50187FAC-F2B5-5042-AC60-BDB8B0EE9C51}">
   <dimension ref="A1:T93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12091,7 +12074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE399293-5FBA-014E-BCB6-AAB0AC976680}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>

</xml_diff>